<commit_message>
chore: Split scripts and set P2R group up
</commit_message>
<xml_diff>
--- a/NEWREQUIREMENT.xlsx
+++ b/NEWREQUIREMENT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101114992\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101114992\Documents\Research\98Coding\00coderepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9786B3A6-3799-4828-B9F1-3E12A7C0BB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D50AD19-2F26-48D9-8345-04145807ADAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="2460" windowWidth="14655" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30705" yWindow="840" windowWidth="12645" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refactor: Change and organize code
</commit_message>
<xml_diff>
--- a/NEWREQUIREMENT.xlsx
+++ b/NEWREQUIREMENT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101114992\Documents\Research\98Coding\00coderepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D50AD19-2F26-48D9-8345-04145807ADAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA7F7BF-DD9E-4749-B854-604187A081EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="840" windowWidth="12645" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31215" yWindow="945" windowWidth="12645" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,10 +472,19 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
fix: Added the dummy var to trucks' list to unfix sched
</commit_message>
<xml_diff>
--- a/NEWREQUIREMENT.xlsx
+++ b/NEWREQUIREMENT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101114992\Documents\Research\98Coding\00coderepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA7F7BF-DD9E-4749-B854-604187A081EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D60D5A-076D-49F5-9C77-3ECCD6BA8F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31215" yWindow="945" windowWidth="12645" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>44686</v>
       </c>
       <c r="G3" s="2">
-        <v>0.50011574074074072</v>
+        <v>0.50706018518518514</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>